<commit_message>
ccp_add function and ccp_colect function
</commit_message>
<xml_diff>
--- a/data/all_in_one.xlsx
+++ b/data/all_in_one.xlsx
@@ -665,7 +665,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC340"/>
+  <dimension ref="A1:AC344"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28658,6 +28658,352 @@
       <c r="AB340" t="s"/>
       <c r="AC340" t="s"/>
     </row>
+    <row r="341" spans="1:29">
+      <c r="A341" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B341" t="s">
+        <v>28</v>
+      </c>
+      <c r="C341" t="s">
+        <v>34</v>
+      </c>
+      <c r="D341" t="s">
+        <v>30</v>
+      </c>
+      <c r="E341" t="n">
+        <v>504653.1888824402</v>
+      </c>
+      <c r="F341" t="n">
+        <v>16121.75146707938</v>
+      </c>
+      <c r="G341" t="n">
+        <v>2579480.234732701</v>
+      </c>
+      <c r="H341" t="n">
+        <v>5046108.209195848</v>
+      </c>
+      <c r="I341" t="n">
+        <v>5046108.209195848</v>
+      </c>
+      <c r="J341" t="n">
+        <v>0</v>
+      </c>
+      <c r="K341" t="n">
+        <v>0</v>
+      </c>
+      <c r="L341" t="n">
+        <v>0</v>
+      </c>
+      <c r="M341" t="n">
+        <v>5046108.209195848</v>
+      </c>
+      <c r="N341" t="n">
+        <v>0</v>
+      </c>
+      <c r="O341" t="n">
+        <v>2755897.59554814</v>
+      </c>
+      <c r="P341" t="n">
+        <v>764022.3593160097</v>
+      </c>
+      <c r="Q341" t="n">
+        <v>4814684</v>
+      </c>
+      <c r="R341" t="n">
+        <v>6351926</v>
+      </c>
+      <c r="S341" t="n">
+        <v>63136358.12420253</v>
+      </c>
+      <c r="T341" t="n">
+        <v>60364677.56497066</v>
+      </c>
+      <c r="U341" t="n">
+        <v>11</v>
+      </c>
+      <c r="V341" t="n">
+        <v>12</v>
+      </c>
+      <c r="W341" t="n">
+        <v>0</v>
+      </c>
+      <c r="X341" t="s"/>
+      <c r="Y341" t="n">
+        <v>22</v>
+      </c>
+      <c r="Z341" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA341" t="n">
+        <v>11932872.98360656</v>
+      </c>
+      <c r="AB341" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC341" t="n">
+        <v>42351496.90609522</v>
+      </c>
+    </row>
+    <row r="342" spans="1:29">
+      <c r="A342" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B342" t="s">
+        <v>28</v>
+      </c>
+      <c r="C342" t="s">
+        <v>34</v>
+      </c>
+      <c r="D342" t="s">
+        <v>31</v>
+      </c>
+      <c r="E342" t="n">
+        <v>942879.1900432063</v>
+      </c>
+      <c r="F342" t="n">
+        <v>16121.75146707938</v>
+      </c>
+      <c r="G342" t="n">
+        <v>2579480.234732701</v>
+      </c>
+      <c r="H342" t="n">
+        <v>9428000.257948024</v>
+      </c>
+      <c r="I342" t="n">
+        <v>9428000.257948024</v>
+      </c>
+      <c r="J342" t="n">
+        <v>0</v>
+      </c>
+      <c r="K342" t="n">
+        <v>0</v>
+      </c>
+      <c r="L342" t="n">
+        <v>0</v>
+      </c>
+      <c r="M342" t="n">
+        <v>9428000.257948024</v>
+      </c>
+      <c r="N342" t="n">
+        <v>0</v>
+      </c>
+      <c r="O342" t="n">
+        <v>2455221.719561488</v>
+      </c>
+      <c r="P342" t="n">
+        <v>1426851.958320716</v>
+      </c>
+      <c r="Q342" t="n">
+        <v>17043517</v>
+      </c>
+      <c r="R342" t="n">
+        <v>28397506</v>
+      </c>
+      <c r="S342" t="n">
+        <v>65411808.06437584</v>
+      </c>
+      <c r="T342" t="n">
+        <v>62619609.24421229</v>
+      </c>
+      <c r="U342" t="n">
+        <v>8</v>
+      </c>
+      <c r="V342" t="n">
+        <v>7</v>
+      </c>
+      <c r="W342" t="n">
+        <v>0</v>
+      </c>
+      <c r="X342" t="n">
+        <v>875</v>
+      </c>
+      <c r="Y342" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z342" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA342" t="n">
+        <v>23738.90163934425</v>
+      </c>
+      <c r="AB342" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC342" t="n">
+        <v>26811630.04297515</v>
+      </c>
+    </row>
+    <row r="343" spans="1:29">
+      <c r="A343" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B343" t="s">
+        <v>28</v>
+      </c>
+      <c r="C343" t="s">
+        <v>34</v>
+      </c>
+      <c r="D343" t="s">
+        <v>32</v>
+      </c>
+      <c r="E343" t="n">
+        <v>322964.6449990327</v>
+      </c>
+      <c r="F343" t="n">
+        <v>16121.75146707938</v>
+      </c>
+      <c r="G343" t="n">
+        <v>2579480.234732701</v>
+      </c>
+      <c r="H343" t="n">
+        <v>3229375.285355001</v>
+      </c>
+      <c r="I343" t="n">
+        <v>3229375.285355001</v>
+      </c>
+      <c r="J343" t="n">
+        <v>0</v>
+      </c>
+      <c r="K343" t="n">
+        <v>0</v>
+      </c>
+      <c r="L343" t="n">
+        <v>0</v>
+      </c>
+      <c r="M343" t="n">
+        <v>3229375.285355001</v>
+      </c>
+      <c r="N343" t="n">
+        <v>0</v>
+      </c>
+      <c r="O343" t="s"/>
+      <c r="P343" t="s"/>
+      <c r="Q343" t="n">
+        <v>0</v>
+      </c>
+      <c r="R343" t="n">
+        <v>9787349</v>
+      </c>
+      <c r="S343" t="n">
+        <v>20024435.17669093</v>
+      </c>
+      <c r="T343" t="n">
+        <v>19989468.28851486</v>
+      </c>
+      <c r="U343" t="n">
+        <v>0</v>
+      </c>
+      <c r="V343" t="n">
+        <v>38</v>
+      </c>
+      <c r="W343" t="n">
+        <v>0</v>
+      </c>
+      <c r="X343" t="s"/>
+      <c r="Y343" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z343" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA343" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB343" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC343" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:29">
+      <c r="A344" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B344" t="s">
+        <v>28</v>
+      </c>
+      <c r="C344" t="s">
+        <v>34</v>
+      </c>
+      <c r="D344" t="s">
+        <v>33</v>
+      </c>
+      <c r="E344" t="n">
+        <v>112241.4167795189</v>
+      </c>
+      <c r="F344" t="n">
+        <v>16121.75146707938</v>
+      </c>
+      <c r="G344" t="n">
+        <v>2579480.234732701</v>
+      </c>
+      <c r="H344" t="n">
+        <v>1111000</v>
+      </c>
+      <c r="I344" t="n">
+        <v>1111000</v>
+      </c>
+      <c r="J344" t="n">
+        <v>0</v>
+      </c>
+      <c r="K344" t="n">
+        <v>0</v>
+      </c>
+      <c r="L344" t="n">
+        <v>0</v>
+      </c>
+      <c r="M344" t="n">
+        <v>1111000</v>
+      </c>
+      <c r="N344" t="n">
+        <v>0</v>
+      </c>
+      <c r="O344" t="n">
+        <v>126998.4047359257</v>
+      </c>
+      <c r="P344" t="n">
+        <v>39534.6277334805</v>
+      </c>
+      <c r="Q344" t="n">
+        <v>0</v>
+      </c>
+      <c r="R344" t="n">
+        <v>136000</v>
+      </c>
+      <c r="S344" t="n">
+        <v>13961141.68599544</v>
+      </c>
+      <c r="T344" t="n">
+        <v>13348961.19816857</v>
+      </c>
+      <c r="U344" t="n">
+        <v>0</v>
+      </c>
+      <c r="V344" t="n">
+        <v>24</v>
+      </c>
+      <c r="W344" t="n">
+        <v>0</v>
+      </c>
+      <c r="X344" t="s"/>
+      <c r="Y344" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z344" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA344" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB344" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC344" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>